<commit_message>
Updated protocols with alive signal
</commit_message>
<xml_diff>
--- a/serial_protocols_definition.xlsx
+++ b/serial_protocols_definition.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B48923\Documents\GitHub\DistantIO\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="10440" activeTab="1"/>
   </bookViews>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="109">
   <si>
     <t>command</t>
   </si>
@@ -335,6 +340,18 @@
   </si>
   <si>
     <t>TABLE ENTRIES (see below)</t>
+  </si>
+  <si>
+    <t>MCU AUTONOMOUS SIGNALS</t>
+  </si>
+  <si>
+    <t>frame</t>
+  </si>
+  <si>
+    <t>0x55</t>
+  </si>
+  <si>
+    <t>Alive signal (every 100 ms)</t>
   </si>
 </sst>
 </file>
@@ -619,7 +636,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -672,24 +689,64 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -702,12 +759,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -735,44 +786,47 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1053,7 +1107,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1111,10 +1165,10 @@
       <c r="C11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="31"/>
+      <c r="E11" s="32"/>
       <c r="F11" s="4" t="s">
         <v>11</v>
       </c>
@@ -1342,10 +1396,10 @@
       <c r="B24" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="32"/>
+      <c r="D24" s="33"/>
       <c r="E24" s="15"/>
       <c r="F24" s="23" t="s">
         <v>54</v>
@@ -1361,14 +1415,14 @@
       </c>
       <c r="J24" s="16"/>
       <c r="K24" s="15"/>
-      <c r="L24" s="29" t="s">
+      <c r="L24" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="M24" s="29"/>
-      <c r="N24" s="29"/>
-      <c r="O24" s="29"/>
-      <c r="P24" s="29"/>
-      <c r="Q24" s="29"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="30"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="30"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
@@ -1402,10 +1456,10 @@
     <row r="26" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
       <c r="B26" s="21"/>
-      <c r="C26" s="33" t="s">
+      <c r="C26" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="33"/>
+      <c r="D26" s="34"/>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
       <c r="G26" s="15"/>
@@ -1421,8 +1475,8 @@
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="21"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="15"/>
@@ -1440,22 +1494,22 @@
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
       <c r="B28" s="15"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C30" s="30" t="s">
+      <c r="C30" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="30"/>
+      <c r="D30" s="31"/>
       <c r="F30" s="23" t="s">
         <v>54</v>
       </c>
@@ -1470,38 +1524,38 @@
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
     </row>
     <row r="34" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="30" t="s">
+      <c r="C34" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="D34" s="30"/>
+      <c r="D34" s="31"/>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1519,10 +1573,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:W38"/>
+  <dimension ref="B6:W44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,129 +1585,130 @@
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="E6" s="56" t="s">
+      <c r="E6" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="60" t="s">
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="M6" s="56" t="s">
+      <c r="M6" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="N6" s="56"/>
-      <c r="O6" s="56"/>
-      <c r="P6" s="56"/>
-      <c r="Q6" s="56"/>
-      <c r="R6" s="56"/>
-      <c r="S6" s="56"/>
-      <c r="T6" s="56"/>
-      <c r="U6" s="56"/>
-      <c r="V6" s="56"/>
-      <c r="W6" s="56"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="40"/>
+      <c r="S6" s="40"/>
+      <c r="T6" s="40"/>
+      <c r="U6" s="40"/>
+      <c r="V6" s="40"/>
+      <c r="W6" s="40"/>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="56"/>
-      <c r="L7" s="60"/>
-      <c r="M7" s="56"/>
-      <c r="N7" s="56"/>
-      <c r="O7" s="56"/>
-      <c r="P7" s="56"/>
-      <c r="Q7" s="56"/>
-      <c r="R7" s="56"/>
-      <c r="S7" s="56"/>
-      <c r="T7" s="56"/>
-      <c r="U7" s="56"/>
-      <c r="V7" s="56"/>
-      <c r="W7" s="56"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
+      <c r="S7" s="40"/>
+      <c r="T7" s="40"/>
+      <c r="U7" s="40"/>
+      <c r="V7" s="40"/>
+      <c r="W7" s="40"/>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C8" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="55"/>
-      <c r="E8" s="1" t="s">
+      <c r="C8" s="69" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="70"/>
+      <c r="E8" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="57" t="s">
+      <c r="F8" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="52" t="s">
+      <c r="I8" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="52" t="s">
+      <c r="J8" s="73" t="s">
         <v>65</v>
       </c>
-      <c r="K8" s="52" t="s">
+      <c r="K8" s="73" t="s">
         <v>92</v>
       </c>
       <c r="L8" s="14"/>
-      <c r="M8" s="1" t="s">
+      <c r="M8" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="N8" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O8" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="P8" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="Q8" s="52" t="s">
+      <c r="Q8" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="R8" s="52" t="s">
+      <c r="R8" s="73" t="s">
         <v>65</v>
       </c>
-      <c r="S8" s="52" t="s">
+      <c r="S8" s="73" t="s">
         <v>92</v>
       </c>
-      <c r="T8" s="52" t="s">
+      <c r="T8" s="73" t="s">
         <v>93</v>
       </c>
-      <c r="U8" s="1" t="s">
+      <c r="U8" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="V8" s="28" t="s">
+      <c r="V8" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="W8" s="1" t="s">
+      <c r="W8" s="71" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="51"/>
+      <c r="D9" s="45"/>
       <c r="E9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="54" t="s">
+      <c r="F9" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="58"/>
+      <c r="G9" s="43"/>
       <c r="H9" s="15"/>
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
@@ -1662,35 +1717,35 @@
       <c r="M9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N9" s="59" t="s">
+      <c r="N9" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="O9" s="59"/>
-      <c r="P9" s="62" t="s">
+      <c r="O9" s="37"/>
+      <c r="P9" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="Q9" s="62"/>
-      <c r="R9" s="62"/>
-      <c r="S9" s="62"/>
-      <c r="T9" s="63" t="s">
+      <c r="Q9" s="36"/>
+      <c r="R9" s="36"/>
+      <c r="S9" s="36"/>
+      <c r="T9" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="U9" s="63"/>
-      <c r="V9" s="63"/>
-      <c r="W9" s="63"/>
+      <c r="U9" s="38"/>
+      <c r="V9" s="38"/>
+      <c r="W9" s="38"/>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C10" s="50" t="s">
+      <c r="C10" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="D10" s="51"/>
+      <c r="D10" s="45"/>
       <c r="E10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="59" t="s">
+      <c r="F10" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="59"/>
+      <c r="G10" s="37"/>
       <c r="H10" s="39" t="s">
         <v>101</v>
       </c>
@@ -1712,10 +1767,10 @@
       <c r="W10" s="14"/>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="D11" s="51"/>
+      <c r="D11" s="45"/>
       <c r="E11" s="6" t="s">
         <v>26</v>
       </c>
@@ -1729,31 +1784,31 @@
       <c r="M11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="N11" s="61" t="s">
+      <c r="N11" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="O11" s="61"/>
-      <c r="P11" s="61"/>
-      <c r="Q11" s="61"/>
-      <c r="R11" s="61"/>
-      <c r="S11" s="61"/>
-      <c r="T11" s="61"/>
-      <c r="U11" s="61"/>
-      <c r="V11" s="61"/>
-      <c r="W11" s="61"/>
+      <c r="O11" s="35"/>
+      <c r="P11" s="35"/>
+      <c r="Q11" s="35"/>
+      <c r="R11" s="35"/>
+      <c r="S11" s="35"/>
+      <c r="T11" s="35"/>
+      <c r="U11" s="35"/>
+      <c r="V11" s="35"/>
+      <c r="W11" s="35"/>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C12" s="50" t="s">
+      <c r="C12" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="D12" s="51"/>
+      <c r="D12" s="45"/>
       <c r="E12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="59" t="s">
+      <c r="F12" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="59"/>
+      <c r="G12" s="37"/>
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
       <c r="J12" s="15"/>
@@ -1763,10 +1818,10 @@
       </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C13" s="50" t="s">
+      <c r="C13" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="D13" s="51"/>
+      <c r="D13" s="45"/>
       <c r="E13" s="6" t="s">
         <v>28</v>
       </c>
@@ -1781,339 +1836,451 @@
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="M15" s="62" t="s">
+        <v>105</v>
+      </c>
+      <c r="N15" s="63"/>
+      <c r="O15" s="63"/>
+      <c r="P15" s="63"/>
+      <c r="Q15" s="63"/>
+      <c r="R15" s="63"/>
+      <c r="S15" s="63"/>
+      <c r="T15" s="63"/>
+      <c r="U15" s="63"/>
+      <c r="V15" s="63"/>
+      <c r="W15" s="64"/>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B16" s="14"/>
-      <c r="I16" s="3" t="s">
+      <c r="C16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="M16" s="65"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="61"/>
+      <c r="P16" s="61"/>
+      <c r="Q16" s="61"/>
+      <c r="R16" s="61"/>
+      <c r="S16" s="61"/>
+      <c r="T16" s="61"/>
+      <c r="U16" s="61"/>
+      <c r="V16" s="61"/>
+      <c r="W16" s="66"/>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B17" s="14"/>
+      <c r="C17" s="75" t="s">
+        <v>106</v>
+      </c>
+      <c r="D17" s="75"/>
+      <c r="E17" s="14"/>
+      <c r="M17" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="N17" s="67"/>
+      <c r="O17" s="67"/>
+      <c r="P17" s="67"/>
+      <c r="Q17" s="67"/>
+      <c r="R17" s="67"/>
+      <c r="S17" s="67"/>
+      <c r="T17" s="67"/>
+      <c r="U17" s="67"/>
+      <c r="V17" s="67"/>
+      <c r="W17" s="67"/>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B18" s="14"/>
+      <c r="C18" s="68" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="68"/>
+      <c r="E18" s="14"/>
+      <c r="M18" s="76" t="s">
+        <v>107</v>
+      </c>
+      <c r="N18" s="67"/>
+      <c r="O18" s="67"/>
+      <c r="P18" s="67"/>
+      <c r="Q18" s="67"/>
+      <c r="R18" s="67"/>
+      <c r="S18" s="67"/>
+      <c r="T18" s="67"/>
+      <c r="U18" s="67"/>
+      <c r="V18" s="67"/>
+      <c r="W18" s="67"/>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="M19" s="67"/>
+      <c r="N19" s="67"/>
+      <c r="O19" s="67"/>
+      <c r="P19" s="67"/>
+      <c r="Q19" s="67"/>
+      <c r="R19" s="67"/>
+      <c r="S19" s="67"/>
+      <c r="T19" s="67"/>
+      <c r="U19" s="67"/>
+      <c r="V19" s="67"/>
+      <c r="W19" s="67"/>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="E20" s="14"/>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B21" s="14"/>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B22" s="14"/>
+      <c r="I22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="J22" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K16" s="39" t="s">
+      <c r="K22" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="L16" s="39"/>
-      <c r="M16" s="5" t="s">
+      <c r="L22" s="39"/>
+      <c r="M22" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="O16" s="47" t="s">
+      <c r="O22" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="P16" s="35" t="s">
+      <c r="P22" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="Q16" s="36"/>
-      <c r="R16" s="36"/>
-      <c r="S16" s="37"/>
-    </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="14"/>
-      <c r="I17" s="3" t="s">
+      <c r="Q22" s="50"/>
+      <c r="R22" s="50"/>
+      <c r="S22" s="51"/>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B23" s="14"/>
+      <c r="I23" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="J23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K17" s="38" t="s">
+      <c r="K23" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="L17" s="38"/>
-      <c r="M17" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="N17" t="s">
-        <v>86</v>
-      </c>
-      <c r="O17" s="48"/>
-      <c r="P17" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q17" s="41"/>
-      <c r="R17" s="41"/>
-      <c r="S17" s="42"/>
-    </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B18" s="14"/>
-      <c r="I18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K18" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="L18" s="38"/>
-      <c r="M18" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="I19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K19" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="L19" s="38"/>
-      <c r="M19" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="N19" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="I20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K20" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="L20" s="38"/>
-      <c r="M20" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="N20" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="I21" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K21" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="L21" s="38"/>
-      <c r="M21" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="I22" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K22" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="L22" s="38"/>
-      <c r="M22" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="I23" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K23" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="L23" s="38"/>
+      <c r="L23" s="47"/>
       <c r="M23" s="5" t="s">
         <v>49</v>
       </c>
       <c r="N23" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="43"/>
-      <c r="L24" s="44"/>
-      <c r="M24" s="5"/>
-    </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
+      <c r="O23" s="60"/>
+      <c r="P23" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q23" s="53"/>
+      <c r="R23" s="53"/>
+      <c r="S23" s="54"/>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B24" s="14"/>
+      <c r="I24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K24" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="L24" s="47"/>
+      <c r="M24" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="I25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K25" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="L25" s="47"/>
+      <c r="M25" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="N25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="I26" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K26" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="L26" s="47"/>
+      <c r="M26" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="I27" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K27" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="L27" s="47"/>
+      <c r="M27" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="I28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K28" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="L28" s="47"/>
+      <c r="M28" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="I29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K29" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="L29" s="47"/>
+      <c r="M29" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="55"/>
+      <c r="L30" s="56"/>
+      <c r="M30" s="5"/>
+    </row>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E26" s="27" t="s">
+    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="E32" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="F26" s="27"/>
-      <c r="I26" s="53" t="s">
+      <c r="F32" s="27"/>
+      <c r="I32" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="J26" s="53" t="s">
+      <c r="J32" s="28" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E27" s="27" t="s">
+    <row r="33" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="E33" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F27" s="27" t="s">
+      <c r="F33" s="27" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="D28" s="49" t="s">
+    <row r="34" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="D34" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="E28" s="27" t="s">
+      <c r="E34" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="F28" s="27" t="s">
+      <c r="F34" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G34" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="D29" s="49"/>
-      <c r="E29" s="27" t="s">
+    <row r="35" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="D35" s="46"/>
+      <c r="E35" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="F29" s="27" t="s">
+      <c r="F35" s="27" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="D30" s="49"/>
-      <c r="E30" s="27" t="s">
+    <row r="36" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="D36" s="46"/>
+      <c r="E36" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="F30" s="27" t="s">
+      <c r="F36" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="J30" s="46" t="s">
+      <c r="J36" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="K30" s="46"/>
-      <c r="L30" s="26" t="s">
+      <c r="K36" s="58"/>
+      <c r="L36" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="M30" s="26" t="s">
+      <c r="M36" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="N30" s="26" t="s">
+      <c r="N36" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="O30" s="26" t="s">
+      <c r="O36" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="P30" s="26" t="s">
+      <c r="P36" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="Q30" s="26" t="s">
+      <c r="Q36" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="R30" s="26" t="s">
+      <c r="R36" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="S30" s="26" t="s">
+      <c r="S36" s="26" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C31" s="7"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="27" t="s">
+    <row r="37" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C37" s="7"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="F31" s="27" t="s">
+      <c r="F37" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="J31" s="46"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="26" t="s">
+      <c r="J37" s="58"/>
+      <c r="K37" s="58"/>
+      <c r="L37" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="M31" s="45" t="s">
+      <c r="M37" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="N31" s="45"/>
-      <c r="O31" s="45" t="s">
+      <c r="N37" s="57"/>
+      <c r="O37" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="P31" s="45"/>
-      <c r="Q31" s="26" t="s">
+      <c r="P37" s="57"/>
+      <c r="Q37" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="R31" s="26" t="s">
+      <c r="R37" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="S31" s="26" t="s">
+      <c r="S37" s="26" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E32" s="27" t="s">
+    <row r="38" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="E38" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="F32" s="27" t="s">
+      <c r="F38" s="27" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="5:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E33" s="27" t="s">
+    <row r="39" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E39" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="F33" s="27" t="s">
+      <c r="F39" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="L33" s="34" t="s">
+      <c r="L39" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="M33" s="34"/>
-      <c r="O33" s="18"/>
-    </row>
-    <row r="34" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E34" s="27" t="s">
+      <c r="M39" s="48"/>
+      <c r="O39" s="18"/>
+    </row>
+    <row r="40" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="E40" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="F34" s="27" t="s">
+      <c r="F40" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="L34" s="34"/>
-      <c r="M34" s="34"/>
-      <c r="O34" s="18"/>
-    </row>
-    <row r="35" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="L35" s="34"/>
-      <c r="M35" s="34"/>
-      <c r="O35" s="18"/>
-    </row>
-    <row r="36" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="L36" s="34"/>
-      <c r="M36" s="34"/>
-    </row>
-    <row r="37" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="L37" s="34"/>
-      <c r="M37" s="34"/>
-    </row>
-    <row r="38" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="M38" s="18"/>
-      <c r="N38" s="18"/>
+      <c r="L40" s="48"/>
+      <c r="M40" s="48"/>
+      <c r="O40" s="18"/>
+    </row>
+    <row r="41" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="L41" s="48"/>
+      <c r="M41" s="48"/>
+      <c r="O41" s="18"/>
+    </row>
+    <row r="42" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="L42" s="48"/>
+      <c r="M42" s="48"/>
+    </row>
+    <row r="43" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="L43" s="48"/>
+      <c r="M43" s="48"/>
+    </row>
+    <row r="44" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="M44" s="18"/>
+      <c r="N44" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="N11:W11"/>
-    <mergeCell ref="P9:S9"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="T9:W9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:K10"/>
+  <mergeCells count="37">
+    <mergeCell ref="O37:P37"/>
+    <mergeCell ref="J36:K37"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="M15:W16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="P22:S22"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="P23:S23"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="L39:M43"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M37:N37"/>
     <mergeCell ref="E6:K7"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="F9:G9"/>
@@ -2124,24 +2291,12 @@
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="L33:M37"/>
-    <mergeCell ref="P16:S16"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="P17:S17"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="J30:K31"/>
-    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="N11:W11"/>
+    <mergeCell ref="P9:S9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="T9:W9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:K10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added alive frame to protocol definition
</commit_message>
<xml_diff>
--- a/serial_protocols_definition.xlsx
+++ b/serial_protocols_definition.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="127">
   <si>
     <t>command</t>
   </si>
@@ -383,6 +383,30 @@
   </si>
   <si>
     <t>Payload</t>
+  </si>
+  <si>
+    <t>alive-signal</t>
+  </si>
+  <si>
+    <t>MCU</t>
+  </si>
+  <si>
+    <t>0x11</t>
+  </si>
+  <si>
+    <t>0x13</t>
+  </si>
+  <si>
+    <t>0x14</t>
+  </si>
+  <si>
+    <t>0x15</t>
+  </si>
+  <si>
+    <t>0x16</t>
+  </si>
+  <si>
+    <t>0x17</t>
   </si>
 </sst>
 </file>
@@ -667,7 +691,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -743,6 +767,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -752,6 +779,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -760,9 +790,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1159,10 +1186,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F7:U12"/>
+  <dimension ref="F7:U13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,27 +1219,27 @@
       <c r="H8" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="I8" s="39" t="s">
+      <c r="I8" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="J8" s="39"/>
+      <c r="J8" s="42"/>
       <c r="K8" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="40" t="s">
+      <c r="L8" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="M8" s="40"/>
-      <c r="N8" s="40"/>
-      <c r="O8" s="40"/>
-      <c r="P8" s="40"/>
-      <c r="Q8" s="40"/>
-      <c r="R8" s="40"/>
-      <c r="S8" s="40"/>
-      <c r="T8" s="41" t="s">
+      <c r="M8" s="43"/>
+      <c r="N8" s="43"/>
+      <c r="O8" s="43"/>
+      <c r="P8" s="43"/>
+      <c r="Q8" s="43"/>
+      <c r="R8" s="43"/>
+      <c r="S8" s="43"/>
+      <c r="T8" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="U8" s="41"/>
+      <c r="U8" s="44"/>
     </row>
     <row r="9" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F9" s="1" t="s">
@@ -1341,6 +1368,52 @@
       </c>
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
+    </row>
+    <row r="13" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>119</v>
+      </c>
+      <c r="G13" t="s">
+        <v>120</v>
+      </c>
+      <c r="H13" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1405,10 +1478,10 @@
       <c r="C11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="D11" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="44"/>
+      <c r="E11" s="48"/>
       <c r="F11" s="4" t="s">
         <v>11</v>
       </c>
@@ -1655,14 +1728,14 @@
       </c>
       <c r="J24" s="16"/>
       <c r="K24" s="15"/>
-      <c r="L24" s="42" t="s">
+      <c r="L24" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="M24" s="42"/>
-      <c r="N24" s="42"/>
-      <c r="O24" s="42"/>
-      <c r="P24" s="42"/>
-      <c r="Q24" s="42"/>
+      <c r="M24" s="46"/>
+      <c r="N24" s="46"/>
+      <c r="O24" s="46"/>
+      <c r="P24" s="46"/>
+      <c r="Q24" s="46"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
@@ -1696,10 +1769,10 @@
     <row r="26" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
       <c r="B26" s="21"/>
-      <c r="C26" s="46" t="s">
+      <c r="C26" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="46"/>
+      <c r="D26" s="49"/>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
       <c r="G26" s="15"/>
@@ -1715,8 +1788,8 @@
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="21"/>
-      <c r="C27" s="46"/>
-      <c r="D27" s="46"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="15"/>
@@ -1734,22 +1807,22 @@
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
       <c r="B28" s="15"/>
-      <c r="C28" s="46"/>
-      <c r="D28" s="46"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C30" s="43" t="s">
+      <c r="C30" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="43"/>
+      <c r="D30" s="47"/>
       <c r="F30" s="23" t="s">
         <v>54</v>
       </c>
@@ -1764,38 +1837,38 @@
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="43"/>
-      <c r="D33" s="43"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="47"/>
     </row>
     <row r="34" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="43" t="s">
+      <c r="C34" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="D34" s="43"/>
+      <c r="D34" s="47"/>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
+      <c r="C35" s="47"/>
+      <c r="D35" s="47"/>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" s="43"/>
-      <c r="D36" s="43"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="47"/>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C37" s="43"/>
-      <c r="D37" s="43"/>
+      <c r="C37" s="47"/>
+      <c r="D37" s="47"/>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C38" s="43"/>
-      <c r="D38" s="43"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1829,58 +1902,58 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="E6" s="71" t="s">
+      <c r="E6" s="74" t="s">
         <v>98</v>
       </c>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
-      <c r="J6" s="71"/>
-      <c r="K6" s="71"/>
-      <c r="L6" s="72" t="s">
+      <c r="F6" s="74"/>
+      <c r="G6" s="74"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="74"/>
+      <c r="L6" s="75" t="s">
         <v>101</v>
       </c>
-      <c r="M6" s="71" t="s">
+      <c r="M6" s="74" t="s">
         <v>99</v>
       </c>
-      <c r="N6" s="71"/>
-      <c r="O6" s="71"/>
-      <c r="P6" s="71"/>
-      <c r="Q6" s="71"/>
-      <c r="R6" s="71"/>
-      <c r="S6" s="71"/>
-      <c r="T6" s="71"/>
-      <c r="U6" s="71"/>
-      <c r="V6" s="71"/>
-      <c r="W6" s="71"/>
+      <c r="N6" s="74"/>
+      <c r="O6" s="74"/>
+      <c r="P6" s="74"/>
+      <c r="Q6" s="74"/>
+      <c r="R6" s="74"/>
+      <c r="S6" s="74"/>
+      <c r="T6" s="74"/>
+      <c r="U6" s="74"/>
+      <c r="V6" s="74"/>
+      <c r="W6" s="74"/>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
-      <c r="L7" s="72"/>
-      <c r="M7" s="71"/>
-      <c r="N7" s="71"/>
-      <c r="O7" s="71"/>
-      <c r="P7" s="71"/>
-      <c r="Q7" s="71"/>
-      <c r="R7" s="71"/>
-      <c r="S7" s="71"/>
-      <c r="T7" s="71"/>
-      <c r="U7" s="71"/>
-      <c r="V7" s="71"/>
-      <c r="W7" s="71"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
+      <c r="O7" s="74"/>
+      <c r="P7" s="74"/>
+      <c r="Q7" s="74"/>
+      <c r="R7" s="74"/>
+      <c r="S7" s="74"/>
+      <c r="T7" s="74"/>
+      <c r="U7" s="74"/>
+      <c r="V7" s="74"/>
+      <c r="W7" s="74"/>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C8" s="77" t="s">
+      <c r="C8" s="80" t="s">
         <v>105</v>
       </c>
-      <c r="D8" s="78"/>
+      <c r="D8" s="81"/>
       <c r="E8" s="31" t="s">
         <v>1</v>
       </c>
@@ -1938,17 +2011,17 @@
       </c>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C9" s="75" t="s">
+      <c r="C9" s="78" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="76"/>
+      <c r="D9" s="79"/>
       <c r="E9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="73" t="s">
+      <c r="F9" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="74"/>
+      <c r="G9" s="77"/>
       <c r="H9" s="15"/>
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
@@ -1957,41 +2030,41 @@
       <c r="M9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N9" s="67" t="s">
+      <c r="N9" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="O9" s="67"/>
-      <c r="P9" s="80" t="s">
+      <c r="O9" s="70"/>
+      <c r="P9" s="83" t="s">
         <v>95</v>
       </c>
-      <c r="Q9" s="80"/>
-      <c r="R9" s="80"/>
-      <c r="S9" s="80"/>
-      <c r="T9" s="81" t="s">
+      <c r="Q9" s="83"/>
+      <c r="R9" s="83"/>
+      <c r="S9" s="83"/>
+      <c r="T9" s="84" t="s">
         <v>94</v>
       </c>
-      <c r="U9" s="81"/>
-      <c r="V9" s="81"/>
-      <c r="W9" s="81"/>
+      <c r="U9" s="84"/>
+      <c r="V9" s="84"/>
+      <c r="W9" s="84"/>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="D10" s="76"/>
+      <c r="D10" s="79"/>
       <c r="E10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="67" t="s">
+      <c r="F10" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="67"/>
-      <c r="H10" s="40" t="s">
+      <c r="G10" s="70"/>
+      <c r="H10" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
       <c r="M10" s="14" t="s">
         <v>102</v>
       </c>
@@ -2007,10 +2080,10 @@
       <c r="W10" s="14"/>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C11" s="75" t="s">
+      <c r="C11" s="78" t="s">
         <v>108</v>
       </c>
-      <c r="D11" s="76"/>
+      <c r="D11" s="79"/>
       <c r="E11" s="6" t="s">
         <v>26</v>
       </c>
@@ -2028,31 +2101,31 @@
       <c r="M11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="N11" s="79" t="s">
+      <c r="N11" s="82" t="s">
         <v>103</v>
       </c>
-      <c r="O11" s="79"/>
-      <c r="P11" s="79"/>
-      <c r="Q11" s="79"/>
-      <c r="R11" s="79"/>
-      <c r="S11" s="79"/>
-      <c r="T11" s="79"/>
-      <c r="U11" s="79"/>
-      <c r="V11" s="79"/>
-      <c r="W11" s="79"/>
+      <c r="O11" s="82"/>
+      <c r="P11" s="82"/>
+      <c r="Q11" s="82"/>
+      <c r="R11" s="82"/>
+      <c r="S11" s="82"/>
+      <c r="T11" s="82"/>
+      <c r="U11" s="82"/>
+      <c r="V11" s="82"/>
+      <c r="W11" s="82"/>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C12" s="75" t="s">
+      <c r="C12" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="D12" s="76"/>
+      <c r="D12" s="79"/>
       <c r="E12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="67" t="s">
+      <c r="F12" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="67"/>
+      <c r="G12" s="70"/>
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
       <c r="J12" s="15"/>
@@ -2062,10 +2135,10 @@
       </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C13" s="75" t="s">
+      <c r="C13" s="78" t="s">
         <v>89</v>
       </c>
-      <c r="D13" s="76"/>
+      <c r="D13" s="79"/>
       <c r="E13" s="6" t="s">
         <v>28</v>
       </c>
@@ -2082,42 +2155,42 @@
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="E15" s="14"/>
-      <c r="M15" s="51" t="s">
+      <c r="M15" s="54" t="s">
         <v>104</v>
       </c>
-      <c r="N15" s="52"/>
-      <c r="O15" s="52"/>
-      <c r="P15" s="52"/>
-      <c r="Q15" s="52"/>
-      <c r="R15" s="52"/>
-      <c r="S15" s="52"/>
-      <c r="T15" s="52"/>
-      <c r="U15" s="52"/>
-      <c r="V15" s="52"/>
-      <c r="W15" s="53"/>
+      <c r="N15" s="55"/>
+      <c r="O15" s="55"/>
+      <c r="P15" s="55"/>
+      <c r="Q15" s="55"/>
+      <c r="R15" s="55"/>
+      <c r="S15" s="55"/>
+      <c r="T15" s="55"/>
+      <c r="U15" s="55"/>
+      <c r="V15" s="55"/>
+      <c r="W15" s="56"/>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
       <c r="E16" s="14"/>
-      <c r="M16" s="54"/>
-      <c r="N16" s="55"/>
-      <c r="O16" s="55"/>
-      <c r="P16" s="55"/>
-      <c r="Q16" s="55"/>
-      <c r="R16" s="55"/>
-      <c r="S16" s="55"/>
-      <c r="T16" s="55"/>
-      <c r="U16" s="55"/>
-      <c r="V16" s="55"/>
-      <c r="W16" s="56"/>
+      <c r="M16" s="57"/>
+      <c r="N16" s="58"/>
+      <c r="O16" s="58"/>
+      <c r="P16" s="58"/>
+      <c r="Q16" s="58"/>
+      <c r="R16" s="58"/>
+      <c r="S16" s="58"/>
+      <c r="T16" s="58"/>
+      <c r="U16" s="58"/>
+      <c r="V16" s="58"/>
+      <c r="W16" s="59"/>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B17" s="14"/>
-      <c r="C17" s="57" t="s">
+      <c r="C17" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="D17" s="57"/>
+      <c r="D17" s="60"/>
       <c r="E17" s="14"/>
       <c r="M17" s="29" t="s">
         <v>1</v>
@@ -2135,10 +2208,10 @@
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
-      <c r="C18" s="58" t="s">
+      <c r="C18" s="61" t="s">
         <v>107</v>
       </c>
-      <c r="D18" s="58"/>
+      <c r="D18" s="61"/>
       <c r="E18" s="14"/>
       <c r="M18" s="35" t="s">
         <v>106</v>
@@ -2186,22 +2259,22 @@
       <c r="J22" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K22" s="40" t="s">
+      <c r="K22" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="L22" s="40"/>
+      <c r="L22" s="43"/>
       <c r="M22" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="O22" s="49" t="s">
+      <c r="O22" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="P22" s="59" t="s">
+      <c r="P22" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="Q22" s="60"/>
-      <c r="R22" s="60"/>
-      <c r="S22" s="61"/>
+      <c r="Q22" s="63"/>
+      <c r="R22" s="63"/>
+      <c r="S22" s="64"/>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B23" s="14"/>
@@ -2211,23 +2284,23 @@
       <c r="J23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K23" s="62" t="s">
+      <c r="K23" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="L23" s="62"/>
+      <c r="L23" s="65"/>
       <c r="M23" s="5" t="s">
         <v>49</v>
       </c>
       <c r="N23" t="s">
         <v>86</v>
       </c>
-      <c r="O23" s="50"/>
-      <c r="P23" s="63" t="s">
+      <c r="O23" s="53"/>
+      <c r="P23" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="Q23" s="64"/>
-      <c r="R23" s="64"/>
-      <c r="S23" s="65"/>
+      <c r="Q23" s="67"/>
+      <c r="R23" s="67"/>
+      <c r="S23" s="68"/>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B24" s="14"/>
@@ -2237,10 +2310,10 @@
       <c r="J24" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K24" s="62" t="s">
+      <c r="K24" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="L24" s="62"/>
+      <c r="L24" s="65"/>
       <c r="M24" s="5" t="s">
         <v>50</v>
       </c>
@@ -2252,10 +2325,10 @@
       <c r="J25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K25" s="62" t="s">
+      <c r="K25" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="L25" s="62"/>
+      <c r="L25" s="65"/>
       <c r="M25" s="5" t="s">
         <v>51</v>
       </c>
@@ -2270,10 +2343,10 @@
       <c r="J26" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K26" s="62" t="s">
+      <c r="K26" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="L26" s="62"/>
+      <c r="L26" s="65"/>
       <c r="M26" s="5" t="s">
         <v>49</v>
       </c>
@@ -2288,10 +2361,10 @@
       <c r="J27" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K27" s="62" t="s">
+      <c r="K27" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="L27" s="62"/>
+      <c r="L27" s="65"/>
       <c r="M27" s="5" t="s">
         <v>50</v>
       </c>
@@ -2303,10 +2376,10 @@
       <c r="J28" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K28" s="62" t="s">
+      <c r="K28" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="L28" s="62"/>
+      <c r="L28" s="65"/>
       <c r="M28" s="5" t="s">
         <v>51</v>
       </c>
@@ -2318,10 +2391,10 @@
       <c r="J29" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K29" s="62" t="s">
+      <c r="K29" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="L29" s="62"/>
+      <c r="L29" s="65"/>
       <c r="M29" s="5" t="s">
         <v>49</v>
       </c>
@@ -2332,8 +2405,8 @@
     <row r="30" spans="2:23" x14ac:dyDescent="0.25">
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
-      <c r="K30" s="69"/>
-      <c r="L30" s="70"/>
+      <c r="K30" s="72"/>
+      <c r="L30" s="73"/>
       <c r="M30" s="5"/>
     </row>
     <row r="31" spans="2:23" x14ac:dyDescent="0.25">
@@ -2362,7 +2435,7 @@
       </c>
     </row>
     <row r="34" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="D34" s="66" t="s">
+      <c r="D34" s="69" t="s">
         <v>69</v>
       </c>
       <c r="E34" s="27" t="s">
@@ -2376,7 +2449,7 @@
       </c>
     </row>
     <row r="35" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="D35" s="66"/>
+      <c r="D35" s="69"/>
       <c r="E35" s="27" t="s">
         <v>73</v>
       </c>
@@ -2385,17 +2458,17 @@
       </c>
     </row>
     <row r="36" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="D36" s="66"/>
+      <c r="D36" s="69"/>
       <c r="E36" s="27" t="s">
         <v>75</v>
       </c>
       <c r="F36" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="J36" s="48" t="s">
+      <c r="J36" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="K36" s="48"/>
+      <c r="K36" s="51"/>
       <c r="L36" s="26" t="s">
         <v>1</v>
       </c>
@@ -2423,26 +2496,26 @@
     </row>
     <row r="37" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C37" s="7"/>
-      <c r="D37" s="66"/>
+      <c r="D37" s="69"/>
       <c r="E37" s="27" t="s">
         <v>78</v>
       </c>
       <c r="F37" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="J37" s="48"/>
-      <c r="K37" s="48"/>
+      <c r="J37" s="51"/>
+      <c r="K37" s="51"/>
       <c r="L37" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="M37" s="47" t="s">
+      <c r="M37" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="N37" s="47"/>
-      <c r="O37" s="47" t="s">
+      <c r="N37" s="50"/>
+      <c r="O37" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="P37" s="47"/>
+      <c r="P37" s="50"/>
       <c r="Q37" s="26" t="s">
         <v>66</v>
       </c>
@@ -2468,10 +2541,10 @@
       <c r="F39" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="L39" s="68" t="s">
+      <c r="L39" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="M39" s="68"/>
+      <c r="M39" s="71"/>
       <c r="O39" s="18"/>
     </row>
     <row r="40" spans="3:19" x14ac:dyDescent="0.25">
@@ -2481,22 +2554,22 @@
       <c r="F40" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="L40" s="68"/>
-      <c r="M40" s="68"/>
+      <c r="L40" s="71"/>
+      <c r="M40" s="71"/>
       <c r="O40" s="18"/>
     </row>
     <row r="41" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="L41" s="68"/>
-      <c r="M41" s="68"/>
+      <c r="L41" s="71"/>
+      <c r="M41" s="71"/>
       <c r="O41" s="18"/>
     </row>
     <row r="42" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="L42" s="68"/>
-      <c r="M42" s="68"/>
+      <c r="L42" s="71"/>
+      <c r="M42" s="71"/>
     </row>
     <row r="43" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="L43" s="68"/>
-      <c r="M43" s="68"/>
+      <c r="L43" s="71"/>
+      <c r="M43" s="71"/>
     </row>
     <row r="44" spans="3:19" x14ac:dyDescent="0.25">
       <c r="M44" s="18"/>

</xml_diff>

<commit_message>
Forgotten changes to commit
</commit_message>
<xml_diff>
--- a/serial_protocols_definition.xlsx
+++ b/serial_protocols_definition.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="10440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="distant IO protocol" sheetId="5" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="90">
   <si>
     <t>byte 0</t>
   </si>
@@ -289,6 +289,12 @@
   </si>
   <si>
     <t>Implementation status</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>uint16</t>
   </si>
 </sst>
 </file>
@@ -374,7 +380,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -386,120 +392,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -548,23 +440,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -579,9 +460,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -603,7 +484,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -619,7 +500,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -628,28 +508,32 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -657,6 +541,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -666,87 +553,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -756,14 +565,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1052,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:V28"/>
+  <dimension ref="A2:X28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,138 +882,148 @@
     <col min="12" max="12" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="83" t="s">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="E2" s="46" t="s">
+      <c r="B2" s="42"/>
+      <c r="E2" s="59" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="47"/>
-      <c r="S2" s="47"/>
-      <c r="T2" s="47"/>
-      <c r="U2" s="47"/>
-      <c r="V2" s="47"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="59"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="59"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="73" t="s">
+      <c r="F3" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="73"/>
-      <c r="H3" s="41" t="s">
+      <c r="G3" s="43"/>
+      <c r="H3" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="76" t="s">
+      <c r="I3" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="J3" s="77"/>
-      <c r="K3" s="78" t="s">
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="L3" s="79"/>
-      <c r="M3" s="74" t="s">
+      <c r="N3" s="61"/>
+      <c r="O3" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="N3" s="74"/>
-      <c r="O3" s="74"/>
-      <c r="P3" s="74"/>
-      <c r="Q3" s="74"/>
-      <c r="R3" s="74"/>
-      <c r="S3" s="74"/>
-      <c r="T3" s="74"/>
-      <c r="U3" s="75" t="s">
+      <c r="P3" s="44"/>
+      <c r="Q3" s="44"/>
+      <c r="R3" s="44"/>
+      <c r="S3" s="44"/>
+      <c r="T3" s="44"/>
+      <c r="U3" s="44"/>
+      <c r="V3" s="44"/>
+      <c r="W3" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="V3" s="75"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X3" s="45"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C4" s="27" t="s">
         <v>44</v>
       </c>
       <c r="D4" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="34">
+      <c r="E4" s="33">
         <v>0</v>
       </c>
-      <c r="F4" s="35">
+      <c r="F4" s="34">
         <v>1</v>
       </c>
-      <c r="G4" s="35">
+      <c r="G4" s="34">
         <v>2</v>
       </c>
-      <c r="H4" s="42">
+      <c r="H4" s="39">
         <v>3</v>
       </c>
-      <c r="I4" s="34">
+      <c r="I4" s="33">
         <v>4</v>
       </c>
-      <c r="J4" s="34">
+      <c r="J4" s="33">
         <v>5</v>
       </c>
-      <c r="K4" s="39">
+      <c r="K4" s="33">
         <v>6</v>
       </c>
-      <c r="L4" s="39">
+      <c r="L4" s="33">
         <v>7</v>
       </c>
-      <c r="M4" s="36">
+      <c r="M4" s="37">
         <v>8</v>
       </c>
-      <c r="N4" s="36">
+      <c r="N4" s="37">
         <v>9</v>
       </c>
-      <c r="O4" s="36">
+      <c r="O4" s="35">
         <v>10</v>
       </c>
-      <c r="P4" s="36">
+      <c r="P4" s="35">
         <v>11</v>
       </c>
-      <c r="Q4" s="36">
+      <c r="Q4" s="35">
         <v>12</v>
       </c>
-      <c r="R4" s="36">
+      <c r="R4" s="35">
         <v>13</v>
       </c>
-      <c r="S4" s="37">
+      <c r="S4" s="35">
         <v>14</v>
       </c>
-      <c r="T4" s="37">
+      <c r="T4" s="35">
         <v>15</v>
       </c>
-      <c r="U4" s="40">
+      <c r="U4" s="35">
         <v>16</v>
       </c>
-      <c r="V4" s="40">
+      <c r="V4" s="35">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W4" s="58">
+        <v>18</v>
+      </c>
+      <c r="X4" s="58">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="26"/>
       <c r="B5" s="26"/>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="31" t="s">
         <v>52</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1206,11 +1032,11 @@
       <c r="E5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="64" t="s">
+      <c r="F5" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="G5" s="65"/>
-      <c r="H5" s="68" t="s">
+      <c r="G5" s="53"/>
+      <c r="H5" s="46" t="s">
         <v>70</v>
       </c>
       <c r="I5" s="50" t="s">
@@ -1227,15 +1053,17 @@
       <c r="R5" s="50"/>
       <c r="S5" s="50"/>
       <c r="T5" s="50"/>
-      <c r="U5" s="44" t="s">
+      <c r="U5" s="50"/>
+      <c r="V5" s="50"/>
+      <c r="W5" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="V5" s="45"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X5" s="62"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="26"/>
       <c r="B6" s="26"/>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="31" t="s">
         <v>55</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1244,36 +1072,38 @@
       <c r="E6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="66"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="48" t="s">
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="J6" s="48"/>
-      <c r="K6" s="49" t="s">
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="L6" s="49"/>
-      <c r="M6" s="70" t="s">
+      <c r="N6" s="48"/>
+      <c r="O6" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="N6" s="71"/>
-      <c r="O6" s="71"/>
-      <c r="P6" s="71"/>
-      <c r="Q6" s="71"/>
-      <c r="R6" s="71"/>
-      <c r="S6" s="71"/>
-      <c r="T6" s="72"/>
-      <c r="U6" s="44" t="s">
+      <c r="P6" s="50"/>
+      <c r="Q6" s="50"/>
+      <c r="R6" s="50"/>
+      <c r="S6" s="50"/>
+      <c r="T6" s="50"/>
+      <c r="U6" s="50"/>
+      <c r="V6" s="50"/>
+      <c r="W6" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="V6" s="45"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X6" s="62"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="26"/>
       <c r="B7" s="26"/>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="31" t="s">
         <v>45</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1282,38 +1112,42 @@
       <c r="E7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="53" t="s">
+      <c r="F7" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="G7" s="54"/>
-      <c r="H7" s="57" t="s">
+      <c r="G7" s="51"/>
+      <c r="H7" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="I7" s="53" t="s">
+      <c r="I7" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="J7" s="59"/>
-      <c r="K7" s="59"/>
-      <c r="L7" s="54"/>
-      <c r="M7" s="53" t="s">
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="51"/>
+      <c r="M7" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="N7" s="59"/>
-      <c r="O7" s="59"/>
-      <c r="P7" s="59"/>
-      <c r="Q7" s="59"/>
-      <c r="R7" s="59"/>
-      <c r="S7" s="59"/>
-      <c r="T7" s="54"/>
-      <c r="U7" s="44" t="s">
+      <c r="N7" s="51"/>
+      <c r="O7" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="P7" s="51"/>
+      <c r="Q7" s="51"/>
+      <c r="R7" s="51"/>
+      <c r="S7" s="51"/>
+      <c r="T7" s="51"/>
+      <c r="U7" s="51"/>
+      <c r="V7" s="51"/>
+      <c r="W7" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="V7" s="45"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X7" s="62"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="26"/>
       <c r="B8" s="26"/>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="31" t="s">
         <v>51</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1322,30 +1156,32 @@
       <c r="E8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="55"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="60"/>
-      <c r="L8" s="56"/>
-      <c r="M8" s="55"/>
-      <c r="N8" s="60"/>
-      <c r="O8" s="60"/>
-      <c r="P8" s="60"/>
-      <c r="Q8" s="60"/>
-      <c r="R8" s="60"/>
-      <c r="S8" s="60"/>
-      <c r="T8" s="56"/>
-      <c r="U8" s="44" t="s">
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="51"/>
+      <c r="O8" s="51"/>
+      <c r="P8" s="51"/>
+      <c r="Q8" s="51"/>
+      <c r="R8" s="51"/>
+      <c r="S8" s="51"/>
+      <c r="T8" s="51"/>
+      <c r="U8" s="51"/>
+      <c r="V8" s="51"/>
+      <c r="W8" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="V8" s="45"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X8" s="62"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="26"/>
       <c r="B9" s="26"/>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="31" t="s">
         <v>57</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1354,11 +1190,11 @@
       <c r="E9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="61" t="s">
+      <c r="F9" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="G9" s="61"/>
-      <c r="H9" s="63" t="s">
+      <c r="G9" s="53"/>
+      <c r="H9" s="46" t="s">
         <v>70</v>
       </c>
       <c r="I9" s="51" t="s">
@@ -1367,25 +1203,29 @@
       <c r="J9" s="51"/>
       <c r="K9" s="51"/>
       <c r="L9" s="51"/>
-      <c r="M9" s="50" t="s">
+      <c r="M9" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="N9" s="51"/>
+      <c r="O9" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="N9" s="50"/>
-      <c r="O9" s="50"/>
       <c r="P9" s="50"/>
       <c r="Q9" s="50"/>
       <c r="R9" s="50"/>
       <c r="S9" s="50"/>
       <c r="T9" s="50"/>
-      <c r="U9" s="44" t="s">
+      <c r="U9" s="50"/>
+      <c r="V9" s="50"/>
+      <c r="W9" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="V9" s="45"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X9" s="62"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="26"/>
       <c r="B10" s="26"/>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="32" t="s">
         <v>59</v>
       </c>
       <c r="D10" s="29" t="s">
@@ -1394,32 +1234,34 @@
       <c r="E10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="63"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="46"/>
       <c r="I10" s="51"/>
       <c r="J10" s="51"/>
       <c r="K10" s="51"/>
       <c r="L10" s="51"/>
-      <c r="M10" s="51" t="s">
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="N10" s="51"/>
-      <c r="O10" s="51"/>
       <c r="P10" s="51"/>
       <c r="Q10" s="51"/>
       <c r="R10" s="51"/>
       <c r="S10" s="51"/>
       <c r="T10" s="51"/>
-      <c r="U10" s="44" t="s">
+      <c r="U10" s="51"/>
+      <c r="V10" s="51"/>
+      <c r="W10" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="V10" s="45"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X10" s="62"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="26"/>
       <c r="B11" s="26"/>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="32" t="s">
         <v>60</v>
       </c>
       <c r="D11" s="29" t="s">
@@ -1428,9 +1270,9 @@
       <c r="E11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="63"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="46"/>
       <c r="I11" s="51"/>
       <c r="J11" s="51"/>
       <c r="K11" s="51"/>
@@ -1443,15 +1285,17 @@
       <c r="R11" s="51"/>
       <c r="S11" s="51"/>
       <c r="T11" s="51"/>
-      <c r="U11" s="44" t="s">
+      <c r="U11" s="51"/>
+      <c r="V11" s="51"/>
+      <c r="W11" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="V11" s="45"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X11" s="62"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="32" t="s">
         <v>71</v>
       </c>
       <c r="D12" s="29" t="s">
@@ -1460,108 +1304,120 @@
       <c r="E12" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="63"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="46"/>
       <c r="I12" s="51"/>
       <c r="J12" s="51"/>
       <c r="K12" s="51"/>
       <c r="L12" s="51"/>
-      <c r="M12" s="50" t="s">
+      <c r="M12" s="51"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="N12" s="50"/>
-      <c r="O12" s="50"/>
       <c r="P12" s="50"/>
       <c r="Q12" s="50"/>
       <c r="R12" s="50"/>
       <c r="S12" s="50"/>
       <c r="T12" s="50"/>
-      <c r="U12" s="44" t="s">
+      <c r="U12" s="50"/>
+      <c r="V12" s="50"/>
+      <c r="W12" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="V12" s="45"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X12" s="62"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="26"/>
       <c r="B13" s="26"/>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="32" t="s">
         <v>72</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="63"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="46"/>
       <c r="I13" s="51"/>
       <c r="J13" s="51"/>
       <c r="K13" s="51"/>
       <c r="L13" s="51"/>
-      <c r="M13" s="52" t="s">
+      <c r="M13" s="51"/>
+      <c r="N13" s="51"/>
+      <c r="O13" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="N13" s="52"/>
-      <c r="O13" s="52"/>
       <c r="P13" s="52"/>
       <c r="Q13" s="52"/>
       <c r="R13" s="52"/>
       <c r="S13" s="52"/>
       <c r="T13" s="52"/>
-      <c r="U13" s="44" t="s">
+      <c r="U13" s="52"/>
+      <c r="V13" s="52"/>
+      <c r="W13" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="V13" s="45"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X13" s="62"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
       <c r="B14" s="26"/>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="32" t="s">
         <v>75</v>
       </c>
       <c r="D14" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F14" s="62" t="s">
+      <c r="F14" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="G14" s="62"/>
-      <c r="H14" s="63"/>
-      <c r="I14" s="48" t="s">
+      <c r="G14" s="49"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="J14" s="48"/>
-      <c r="K14" s="49" t="s">
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="L14" s="49"/>
-      <c r="M14" s="50" t="s">
+      <c r="N14" s="48"/>
+      <c r="O14" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="N14" s="50"/>
-      <c r="O14" s="50"/>
       <c r="P14" s="50"/>
       <c r="Q14" s="50"/>
       <c r="R14" s="50"/>
       <c r="S14" s="50"/>
       <c r="T14" s="50"/>
-      <c r="U14" s="44" t="s">
+      <c r="U14" s="50"/>
+      <c r="V14" s="50"/>
+      <c r="W14" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="V14" s="45"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="F16" s="62" t="s">
+      <c r="X14" s="62"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F16" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="G16" s="62"/>
-      <c r="H16" s="62"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
+      <c r="L16" t="s">
+        <v>88</v>
+      </c>
+      <c r="N16" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="17" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F17" s="28" t="s">
@@ -1586,118 +1442,120 @@
       </c>
     </row>
     <row r="20" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="I20" s="43" t="s">
+      <c r="I20" s="40" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="21" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H21" s="43" t="s">
+      <c r="H21" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="43" t="s">
+      <c r="I21" s="40" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H22" s="43" t="s">
+      <c r="H22" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="I22" s="43" t="s">
+      <c r="I22" s="40" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H23" s="43" t="s">
+      <c r="H23" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="I23" s="43" t="s">
+      <c r="I23" s="40" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="24" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H24" s="43" t="s">
+      <c r="H24" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="I24" s="43" t="s">
+      <c r="I24" s="40" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="25" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H25" s="43" t="s">
+      <c r="H25" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="I25" s="43" t="s">
+      <c r="I25" s="40" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="26" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H26" s="43" t="s">
+      <c r="H26" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="I26" s="43" t="s">
+      <c r="I26" s="40" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="27" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H27" s="43" t="s">
+      <c r="H27" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="I27" s="43" t="s">
+      <c r="I27" s="40" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="28" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="H28" s="43" t="s">
+      <c r="H28" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="I28" s="43" t="s">
+      <c r="I28" s="40" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="M3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="H9:H14"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="M9:T9"/>
-    <mergeCell ref="F5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="M6:T6"/>
-    <mergeCell ref="I5:T5"/>
-    <mergeCell ref="E2:V2"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="M14:T14"/>
-    <mergeCell ref="M10:T11"/>
-    <mergeCell ref="M12:T12"/>
-    <mergeCell ref="M13:T13"/>
-    <mergeCell ref="F7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:L8"/>
-    <mergeCell ref="M7:T8"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="U6:V6"/>
+  <mergeCells count="41">
     <mergeCell ref="F9:G13"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="I9:L13"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="W12:X12"/>
+    <mergeCell ref="W13:X13"/>
+    <mergeCell ref="W14:X14"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="W10:X10"/>
+    <mergeCell ref="W11:X11"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="M9:N13"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:L8"/>
+    <mergeCell ref="O7:V8"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="I5:V5"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="M7:N8"/>
+    <mergeCell ref="H9:H14"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="O9:V9"/>
+    <mergeCell ref="F5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="O6:V6"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="O14:V14"/>
+    <mergeCell ref="O10:V11"/>
+    <mergeCell ref="O12:V12"/>
+    <mergeCell ref="O13:V13"/>
+    <mergeCell ref="F7:G8"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="O3:V3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="E2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1756,10 +1614,10 @@
       <c r="C11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="82" t="s">
+      <c r="D11" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="82"/>
+      <c r="E11" s="56"/>
       <c r="F11" s="4" t="s">
         <v>10</v>
       </c>
@@ -1987,10 +1845,10 @@
       <c r="B24" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="83" t="s">
+      <c r="C24" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="83"/>
+      <c r="D24" s="42"/>
       <c r="E24" s="15"/>
       <c r="F24" s="23" t="s">
         <v>35</v>
@@ -2006,14 +1864,14 @@
       </c>
       <c r="J24" s="16"/>
       <c r="K24" s="15"/>
-      <c r="L24" s="80" t="s">
+      <c r="L24" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="M24" s="80"/>
-      <c r="N24" s="80"/>
-      <c r="O24" s="80"/>
-      <c r="P24" s="80"/>
-      <c r="Q24" s="80"/>
+      <c r="M24" s="54"/>
+      <c r="N24" s="54"/>
+      <c r="O24" s="54"/>
+      <c r="P24" s="54"/>
+      <c r="Q24" s="54"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
@@ -2047,10 +1905,10 @@
     <row r="26" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
       <c r="B26" s="21"/>
-      <c r="C26" s="84" t="s">
+      <c r="C26" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="84"/>
+      <c r="D26" s="57"/>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
       <c r="G26" s="15"/>
@@ -2066,8 +1924,8 @@
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="21"/>
-      <c r="C27" s="84"/>
-      <c r="D27" s="84"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="15"/>
@@ -2085,22 +1943,22 @@
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
       <c r="B28" s="15"/>
-      <c r="C28" s="84"/>
-      <c r="D28" s="84"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="57"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C29" s="84"/>
-      <c r="D29" s="84"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C30" s="81" t="s">
+      <c r="C30" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="81"/>
+      <c r="D30" s="55"/>
       <c r="F30" s="23" t="s">
         <v>35</v>
       </c>
@@ -2115,38 +1973,38 @@
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C31" s="81"/>
-      <c r="D31" s="81"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="55"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C32" s="81"/>
-      <c r="D32" s="81"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="55"/>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="81"/>
-      <c r="D33" s="81"/>
+      <c r="C33" s="55"/>
+      <c r="D33" s="55"/>
     </row>
     <row r="34" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="81" t="s">
+      <c r="C34" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="D34" s="81"/>
+      <c r="D34" s="55"/>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C35" s="81"/>
-      <c r="D35" s="81"/>
+      <c r="C35" s="55"/>
+      <c r="D35" s="55"/>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" s="81"/>
-      <c r="D36" s="81"/>
+      <c r="C36" s="55"/>
+      <c r="D36" s="55"/>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C37" s="81"/>
-      <c r="D37" s="81"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="55"/>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C38" s="81"/>
-      <c r="D38" s="81"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>